<commit_message>
did survey age compe for 2 sex models
</commit_message>
<xml_diff>
--- a/Things to update for sex model.xlsx
+++ b/Things to update for sex model.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
   <si>
     <t>Object</t>
   </si>
@@ -128,13 +128,58 @@
     <t>suit_main</t>
   </si>
   <si>
-    <t>Bigger things</t>
-  </si>
-  <si>
     <t>srv_comp_hat</t>
   </si>
   <si>
     <t>fsh_comp_hat</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>empirical selectivity</t>
+  </si>
+  <si>
+    <t>composition data</t>
+  </si>
+  <si>
+    <t>combined/separate switches</t>
+  </si>
+  <si>
+    <t>sex in 4th column</t>
+  </si>
+  <si>
+    <t>srv_biom</t>
+  </si>
+  <si>
+    <t>fsh_biom</t>
+  </si>
+  <si>
+    <t>remove sex column</t>
+  </si>
+  <si>
+    <t>control</t>
+  </si>
+  <si>
+    <t>nsex in 5th row</t>
+  </si>
+  <si>
+    <t>R_sexr in 7th</t>
+  </si>
+  <si>
+    <t>SSB_wt_index in 12</t>
+  </si>
+  <si>
+    <t>spawn mo in 6</t>
+  </si>
+  <si>
+    <t>data structure changes</t>
+  </si>
+  <si>
+    <t>Questions</t>
+  </si>
+  <si>
+    <t>sex ratio in the likelihood?</t>
   </si>
 </sst>
 </file>
@@ -461,13 +506,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E32"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -476,9 +524,7 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -487,9 +533,6 @@
       <c r="B2" t="s">
         <v>25</v>
       </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -498,8 +541,8 @@
       <c r="B3" t="s">
         <v>25</v>
       </c>
-      <c r="E3" t="s">
-        <v>36</v>
+      <c r="E3" s="1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -510,7 +553,7 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -551,116 +594,200 @@
       <c r="A10" t="s">
         <v>10</v>
       </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
+      <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
+      <c r="B15" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>37</v>
+      </c>
+      <c r="F22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>41</v>
+      </c>
+      <c r="F23" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>42</v>
+      </c>
+      <c r="F24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>26</v>
       </c>
       <c r="B25" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F27" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F28" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
still wroking on 2 sex model
</commit_message>
<xml_diff>
--- a/Things to update for sex model.xlsx
+++ b/Things to update for sex model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27030" windowHeight="10710"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23850" windowHeight="10515"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
   <si>
     <t>Object</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>sex ratio in the likelihood?</t>
+  </si>
+  <si>
+    <t>added sex column</t>
+  </si>
+  <si>
+    <t>LbyAge</t>
+  </si>
+  <si>
+    <t>ConsumAge</t>
+  </si>
+  <si>
+    <t>Combined fsh_control and srv_control to Fleet_control</t>
+  </si>
+  <si>
+    <t>Combined empirical selectivity</t>
+  </si>
+  <si>
+    <t>Combined fsh_comp and srv_comp</t>
   </si>
 </sst>
 </file>
@@ -506,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -568,6 +586,9 @@
       <c r="A6" t="s">
         <v>6</v>
       </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -776,20 +797,51 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
+      <c r="E29" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>31</v>
       </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>32</v>
       </c>
+      <c r="E31" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>33</v>
+      </c>
+      <c r="E32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>53</v>
+      </c>
+      <c r="E33" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
compiles does not opt
</commit_message>
<xml_diff>
--- a/Things to update for sex model.xlsx
+++ b/Things to update for sex model.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
   <si>
     <t>Object</t>
   </si>
@@ -198,6 +198,18 @@
   </si>
   <si>
     <t>Combined fsh_comp and srv_comp</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>selectivity liv</t>
+  </si>
+  <si>
+    <t>Todo</t>
+  </si>
+  <si>
+    <t>selectivity likelihood is wonky</t>
   </si>
 </sst>
 </file>
@@ -524,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,7 +547,7 @@
     <col min="1" max="1" width="19.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +556,7 @@
       </c>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -552,7 +564,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -563,7 +575,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -574,7 +586,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -582,7 +594,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -590,12 +602,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -603,7 +615,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -611,7 +623,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -621,8 +633,11 @@
       <c r="E10" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -632,8 +647,11 @@
       <c r="E11" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -644,7 +662,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -655,7 +673,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -666,7 +684,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -677,7 +695,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -842,6 +860,16 @@
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E36" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
almost done with 2 sex model, need to update stomachn content
</commit_message>
<xml_diff>
--- a/Things to update for sex model.xlsx
+++ b/Things to update for sex model.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
   <si>
     <t>Object</t>
   </si>
@@ -203,13 +203,64 @@
     <t>M</t>
   </si>
   <si>
-    <t>selectivity liv</t>
-  </si>
-  <si>
     <t>Todo</t>
   </si>
   <si>
     <t>selectivity likelihood is wonky</t>
+  </si>
+  <si>
+    <t>stom_div_bio2</t>
+  </si>
+  <si>
+    <t>of_stomKir</t>
+  </si>
+  <si>
+    <t>suit_other</t>
+  </si>
+  <si>
+    <t>B_eaten</t>
+  </si>
+  <si>
+    <t>othersuit</t>
+  </si>
+  <si>
+    <t>Mn_LatAge</t>
+  </si>
+  <si>
+    <t>ration2Age</t>
+  </si>
+  <si>
+    <t>M2_prop</t>
+  </si>
+  <si>
+    <t>Pmort_ua</t>
+  </si>
+  <si>
+    <t>Added species and sex column to Mn_LatAge</t>
+  </si>
+  <si>
+    <t>added species and sex column</t>
+  </si>
+  <si>
+    <t>eaten_ua</t>
+  </si>
+  <si>
+    <t>eaten_la</t>
+  </si>
+  <si>
+    <t>Need to do</t>
+  </si>
+  <si>
+    <t>Kinzey bits</t>
+  </si>
+  <si>
+    <t>Need to do kinzey bits</t>
+  </si>
+  <si>
+    <t>diet_w_sum</t>
+  </si>
+  <si>
+    <t>diet_w_dat</t>
   </si>
 </sst>
 </file>
@@ -253,9 +304,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +588,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="M23" sqref="M23"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,6 +658,9 @@
       <c r="A7" t="s">
         <v>7</v>
       </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -634,7 +689,7 @@
         <v>39</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -648,7 +703,7 @@
         <v>36</v>
       </c>
       <c r="I11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -726,16 +781,25 @@
       <c r="A19" t="s">
         <v>19</v>
       </c>
+      <c r="B19" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>68</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>21</v>
       </c>
+      <c r="B21" t="s">
+        <v>25</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>49</v>
       </c>
@@ -744,6 +808,9 @@
       <c r="A22" t="s">
         <v>22</v>
       </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
       <c r="E22" t="s">
         <v>37</v>
       </c>
@@ -755,6 +822,9 @@
       <c r="A23" t="s">
         <v>23</v>
       </c>
+      <c r="B23" t="s">
+        <v>25</v>
+      </c>
       <c r="E23" t="s">
         <v>41</v>
       </c>
@@ -766,6 +836,9 @@
       <c r="A24" t="s">
         <v>24</v>
       </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
       <c r="E24" t="s">
         <v>42</v>
       </c>
@@ -799,6 +872,9 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
+      <c r="B27" t="s">
+        <v>25</v>
+      </c>
       <c r="F27" t="s">
         <v>47</v>
       </c>
@@ -807,6 +883,9 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
+      <c r="B28" t="s">
+        <v>25</v>
+      </c>
       <c r="F28" t="s">
         <v>48</v>
       </c>
@@ -815,6 +894,9 @@
       <c r="A29" t="s">
         <v>30</v>
       </c>
+      <c r="B29" t="s">
+        <v>25</v>
+      </c>
       <c r="E29" t="s">
         <v>36</v>
       </c>
@@ -830,7 +912,7 @@
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -845,6 +927,9 @@
       <c r="A32" t="s">
         <v>33</v>
       </c>
+      <c r="B32" t="s">
+        <v>25</v>
+      </c>
       <c r="E32" t="s">
         <v>56</v>
       </c>
@@ -853,6 +938,9 @@
       <c r="A33" t="s">
         <v>53</v>
       </c>
+      <c r="B33" t="s">
+        <v>25</v>
+      </c>
       <c r="E33" t="s">
         <v>57</v>
       </c>
@@ -861,15 +949,124 @@
       <c r="A34" t="s">
         <v>54</v>
       </c>
+      <c r="B34" t="s">
+        <v>25</v>
+      </c>
+      <c r="E34" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>58</v>
       </c>
+      <c r="B35" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
-        <v>59</v>
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>69</v>
+      </c>
+      <c r="B46" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated age trans matrix for 2 sex, updated joint comp likelihood
Updated cpp for joint composition likelihood
Updated ALK for two sexes
updated read/write data
</commit_message>
<xml_diff>
--- a/Things to update for sex model.xlsx
+++ b/Things to update for sex model.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="80">
   <si>
     <t>Object</t>
   </si>
@@ -122,9 +122,6 @@
     <t>UobsWtAge_hat</t>
   </si>
   <si>
-    <t>mn_UobsWtAge_hat</t>
-  </si>
-  <si>
     <t>suit_main</t>
   </si>
   <si>
@@ -261,6 +258,12 @@
   </si>
   <si>
     <t>diet_w_dat</t>
+  </si>
+  <si>
+    <t>get rid of stomtau</t>
+  </si>
+  <si>
+    <t>added sample size to stomach sample, and sexes</t>
   </si>
 </sst>
 </file>
@@ -590,8 +593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +627,7 @@
         <v>25</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -635,7 +638,7 @@
         <v>25</v>
       </c>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -686,10 +689,10 @@
         <v>25</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -700,10 +703,10 @@
         <v>25</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -714,7 +717,7 @@
         <v>25</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -725,7 +728,7 @@
         <v>25</v>
       </c>
       <c r="E13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -736,7 +739,7 @@
         <v>25</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -747,7 +750,7 @@
         <v>25</v>
       </c>
       <c r="E15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -787,7 +790,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B20" t="s">
         <v>25</v>
@@ -801,7 +804,7 @@
         <v>25</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -812,10 +815,10 @@
         <v>25</v>
       </c>
       <c r="E22" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -826,10 +829,10 @@
         <v>25</v>
       </c>
       <c r="E23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,10 +843,10 @@
         <v>25</v>
       </c>
       <c r="E24" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" t="s">
         <v>42</v>
-      </c>
-      <c r="F24" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -854,18 +857,21 @@
         <v>25</v>
       </c>
       <c r="E25" t="s">
+        <v>43</v>
+      </c>
+      <c r="F25" t="s">
         <v>44</v>
-      </c>
-      <c r="F25" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>27</v>
       </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -876,7 +882,7 @@
         <v>25</v>
       </c>
       <c r="F27" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -887,7 +893,7 @@
         <v>25</v>
       </c>
       <c r="F28" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -898,83 +904,95 @@
         <v>25</v>
       </c>
       <c r="E29" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>32</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
       </c>
       <c r="E30" t="s">
         <v>7</v>
       </c>
       <c r="F30" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>32</v>
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
       </c>
       <c r="E31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>33</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
         <v>25</v>
       </c>
       <c r="E32" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B33" t="s">
         <v>25</v>
       </c>
       <c r="E33" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
       </c>
       <c r="E34" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B35" t="s">
         <v>25</v>
+      </c>
+      <c r="E35" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
         <v>25</v>
+      </c>
+      <c r="E36" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B37" t="s">
         <v>25</v>
@@ -982,7 +1000,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
         <v>25</v>
@@ -990,7 +1008,7 @@
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B39" t="s">
         <v>25</v>
@@ -998,47 +1016,34 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B40" t="s">
         <v>25</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="B41" t="s">
         <v>25</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B46" t="s">
         <v>25</v>
@@ -1046,12 +1051,12 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.25">
@@ -1061,12 +1066,12 @@
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>